<commit_message>
Edits to facial animation files
Added new emotions: sad, neutral, and bored. Large code restructuring will occur soon to allow simultaneous triggering of motor and emotion control as well as properly control interrupts between facial emotions.
</commit_message>
<xml_diff>
--- a/Chassis/Face/Face_Accessory_Files/Animation_Code_Generator.xlsx
+++ b/Chassis/Face/Face_Accessory_Files/Animation_Code_Generator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\becca\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\becca\Documents\GitHub\BruinBot-Controls\Chassis\Face\Face_Accessory_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8778937E-11F2-4238-8053-6F1E40FA3C88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBA6D7D-AF90-413E-BE6E-782CA45AE6B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="1905" windowWidth="18900" windowHeight="12375" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>x</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>DRAW FRAMES MIRRORED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type a 1 in each cell where an element should be drawn. Replace cell A21 with the desired color of the drawn shape. Then the red text in cell H34 is the ooutput code which should eb pasted directly in the animation code. </t>
   </si>
 </sst>
 </file>
@@ -1188,8 +1191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U278"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="56" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="56" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1430,6 +1433,9 @@
       <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
       <c r="R9" s="1"/>
+      <c r="U9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="1">
@@ -1530,12 +1536,8 @@
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
-      <c r="I14" s="7">
-        <v>1</v>
-      </c>
-      <c r="J14" s="7">
-        <v>1</v>
-      </c>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
@@ -1690,7 +1692,7 @@
         <v>0</v>
       </c>
       <c r="C23" t="str">
-        <f>IF(B2&gt;0,"m_Matrix.mapLEDXY("&amp;A23&amp;","&amp;B23&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" ref="C23:C38" si="0">IF(B2&gt;0,"m_Matrix.mapLEDXY("&amp;A23&amp;","&amp;B23&amp;","&amp;$A$21&amp;");","")</f>
         <v/>
       </c>
       <c r="H23" t="str">
@@ -1706,7 +1708,7 @@
         <v>1</v>
       </c>
       <c r="C24" t="str">
-        <f>IF(B3&gt;0,"m_Matrix.mapLEDXY("&amp;A24&amp;","&amp;B24&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H24" t="str">
@@ -1722,7 +1724,7 @@
         <v>2</v>
       </c>
       <c r="C25" t="str">
-        <f>IF(B4&gt;0,"m_Matrix.mapLEDXY("&amp;A25&amp;","&amp;B25&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H25" t="str">
@@ -1738,12 +1740,12 @@
         <v>3</v>
       </c>
       <c r="C26" t="str">
-        <f>IF(B5&gt;0,"m_Matrix.mapLEDXY("&amp;A26&amp;","&amp;B26&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H26" t="str">
         <f>CONCATENATE(C123,C124,C125,C126,C127,C128,C129,C130,C131,C132,C133,C134,C135,C136,C137,C138,C139,C140,C141,C142,C143,C144,C145,C146,C147,)</f>
-        <v>m_Matrix.mapLEDXY(7,12,mouthColor);</v>
+        <v/>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.5">
@@ -1754,12 +1756,12 @@
         <v>4</v>
       </c>
       <c r="C27" t="str">
-        <f>IF(B6&gt;0,"m_Matrix.mapLEDXY("&amp;A27&amp;","&amp;B27&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H27" t="str">
         <f>CONCATENATE(C148,C149,C150,C151,C152,C153,C154,C155,C156,C157,C158,C159,C160,C161,C162,C163,C164,C165,C166,C167,C168,C169,C170,C171,C172,)</f>
-        <v>m_Matrix.mapLEDXY(7,13,mouthColor);m_Matrix.mapLEDXY(8,12,mouthColor);m_Matrix.mapLEDXY(8,13,mouthColor);</v>
+        <v>m_Matrix.mapLEDXY(7,13,mouthColor);m_Matrix.mapLEDXY(8,13,mouthColor);</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.5">
@@ -1770,7 +1772,7 @@
         <v>5</v>
       </c>
       <c r="C28" t="str">
-        <f>IF(B7&gt;0,"m_Matrix.mapLEDXY("&amp;A28&amp;","&amp;B28&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H28" t="str">
@@ -1786,7 +1788,7 @@
         <v>6</v>
       </c>
       <c r="C29" t="str">
-        <f>IF(B8&gt;0,"m_Matrix.mapLEDXY("&amp;A29&amp;","&amp;B29&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H29" t="str">
@@ -1802,7 +1804,7 @@
         <v>7</v>
       </c>
       <c r="C30" t="str">
-        <f>IF(B9&gt;0,"m_Matrix.mapLEDXY("&amp;A30&amp;","&amp;B30&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H30" t="str">
@@ -1818,7 +1820,7 @@
         <v>8</v>
       </c>
       <c r="C31" t="str">
-        <f>IF(B10&gt;0,"m_Matrix.mapLEDXY("&amp;A31&amp;","&amp;B31&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H31" t="str">
@@ -1834,7 +1836,7 @@
         <v>9</v>
       </c>
       <c r="C32" t="str">
-        <f>IF(B11&gt;0,"m_Matrix.mapLEDXY("&amp;A32&amp;","&amp;B32&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H32" t="str">
@@ -1850,7 +1852,7 @@
         <v>10</v>
       </c>
       <c r="C33" t="str">
-        <f>IF(B12&gt;0,"m_Matrix.mapLEDXY("&amp;A33&amp;","&amp;B33&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1862,7 +1864,7 @@
         <v>11</v>
       </c>
       <c r="C34" t="str">
-        <f>IF(B13&gt;0,"m_Matrix.mapLEDXY("&amp;A34&amp;","&amp;B34&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G34" s="6" t="s">
@@ -1870,7 +1872,7 @@
       </c>
       <c r="H34" s="4" t="str">
         <f>CONCATENATE(H22,H23,H24,H25,H26,H27,H28,H29,H30,H31,H32)</f>
-        <v>m_Matrix.mapLEDXY(7,12,mouthColor);m_Matrix.mapLEDXY(7,13,mouthColor);m_Matrix.mapLEDXY(8,12,mouthColor);m_Matrix.mapLEDXY(8,13,mouthColor);</v>
+        <v>m_Matrix.mapLEDXY(7,13,mouthColor);m_Matrix.mapLEDXY(8,13,mouthColor);</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.5">
@@ -1881,7 +1883,7 @@
         <v>12</v>
       </c>
       <c r="C35" t="str">
-        <f>IF(B14&gt;0,"m_Matrix.mapLEDXY("&amp;A35&amp;","&amp;B35&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H35" s="5" t="s">
@@ -1896,7 +1898,7 @@
         <v>13</v>
       </c>
       <c r="C36" t="str">
-        <f>IF(B15&gt;0,"m_Matrix.mapLEDXY("&amp;A36&amp;","&amp;B36&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1908,7 +1910,7 @@
         <v>14</v>
       </c>
       <c r="C37" t="str">
-        <f>IF(B16&gt;0,"m_Matrix.mapLEDXY("&amp;A37&amp;","&amp;B37&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1920,7 +1922,7 @@
         <v>15</v>
       </c>
       <c r="C38" t="str">
-        <f>IF(B17&gt;0,"m_Matrix.mapLEDXY("&amp;A38&amp;","&amp;B38&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1932,7 +1934,7 @@
         <v>0</v>
       </c>
       <c r="C39" t="str">
-        <f>IF(C2&gt;0,"m_Matrix.mapLEDXY("&amp;A39&amp;","&amp;B39&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" ref="C39:C54" si="1">IF(C2&gt;0,"m_Matrix.mapLEDXY("&amp;A39&amp;","&amp;B39&amp;","&amp;$A$21&amp;");","")</f>
         <v/>
       </c>
     </row>
@@ -1944,7 +1946,7 @@
         <v>1</v>
       </c>
       <c r="C40" t="str">
-        <f>IF(C3&gt;0,"m_Matrix.mapLEDXY("&amp;A40&amp;","&amp;B40&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1956,7 +1958,7 @@
         <v>2</v>
       </c>
       <c r="C41" t="str">
-        <f>IF(C4&gt;0,"m_Matrix.mapLEDXY("&amp;A41&amp;","&amp;B41&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1968,7 +1970,7 @@
         <v>3</v>
       </c>
       <c r="C42" t="str">
-        <f>IF(C5&gt;0,"m_Matrix.mapLEDXY("&amp;A42&amp;","&amp;B42&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1980,7 +1982,7 @@
         <v>4</v>
       </c>
       <c r="C43" t="str">
-        <f>IF(C6&gt;0,"m_Matrix.mapLEDXY("&amp;A43&amp;","&amp;B43&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1992,7 +1994,7 @@
         <v>5</v>
       </c>
       <c r="C44" t="str">
-        <f>IF(C7&gt;0,"m_Matrix.mapLEDXY("&amp;A44&amp;","&amp;B44&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2004,7 +2006,7 @@
         <v>6</v>
       </c>
       <c r="C45" t="str">
-        <f>IF(C8&gt;0,"m_Matrix.mapLEDXY("&amp;A45&amp;","&amp;B45&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2016,7 +2018,7 @@
         <v>7</v>
       </c>
       <c r="C46" t="str">
-        <f>IF(C9&gt;0,"m_Matrix.mapLEDXY("&amp;A46&amp;","&amp;B46&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2028,7 +2030,7 @@
         <v>8</v>
       </c>
       <c r="C47" t="str">
-        <f>IF(C10&gt;0,"m_Matrix.mapLEDXY("&amp;A47&amp;","&amp;B47&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2040,7 +2042,7 @@
         <v>9</v>
       </c>
       <c r="C48" t="str">
-        <f>IF(C11&gt;0,"m_Matrix.mapLEDXY("&amp;A48&amp;","&amp;B48&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2052,7 +2054,7 @@
         <v>10</v>
       </c>
       <c r="C49" t="str">
-        <f>IF(C12&gt;0,"m_Matrix.mapLEDXY("&amp;A49&amp;","&amp;B49&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2064,7 +2066,7 @@
         <v>11</v>
       </c>
       <c r="C50" t="str">
-        <f>IF(C13&gt;0,"m_Matrix.mapLEDXY("&amp;A50&amp;","&amp;B50&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2076,7 +2078,7 @@
         <v>12</v>
       </c>
       <c r="C51" t="str">
-        <f>IF(C14&gt;0,"m_Matrix.mapLEDXY("&amp;A51&amp;","&amp;B51&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2088,7 +2090,7 @@
         <v>13</v>
       </c>
       <c r="C52" t="str">
-        <f>IF(C15&gt;0,"m_Matrix.mapLEDXY("&amp;A52&amp;","&amp;B52&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2100,7 +2102,7 @@
         <v>14</v>
       </c>
       <c r="C53" t="str">
-        <f>IF(C16&gt;0,"m_Matrix.mapLEDXY("&amp;A53&amp;","&amp;B53&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2112,7 +2114,7 @@
         <v>15</v>
       </c>
       <c r="C54" t="str">
-        <f>IF(C17&gt;0,"m_Matrix.mapLEDXY("&amp;A54&amp;","&amp;B54&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2124,7 +2126,7 @@
         <v>0</v>
       </c>
       <c r="C55" t="str">
-        <f>IF(D2&gt;0,"m_Matrix.mapLEDXY("&amp;A55&amp;","&amp;B55&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" ref="C55:C70" si="2">IF(D2&gt;0,"m_Matrix.mapLEDXY("&amp;A55&amp;","&amp;B55&amp;","&amp;$A$21&amp;");","")</f>
         <v/>
       </c>
     </row>
@@ -2136,7 +2138,7 @@
         <v>1</v>
       </c>
       <c r="C56" t="str">
-        <f>IF(D3&gt;0,"m_Matrix.mapLEDXY("&amp;A56&amp;","&amp;B56&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -2148,7 +2150,7 @@
         <v>2</v>
       </c>
       <c r="C57" t="str">
-        <f>IF(D4&gt;0,"m_Matrix.mapLEDXY("&amp;A57&amp;","&amp;B57&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -2160,7 +2162,7 @@
         <v>3</v>
       </c>
       <c r="C58" t="str">
-        <f>IF(D5&gt;0,"m_Matrix.mapLEDXY("&amp;A58&amp;","&amp;B58&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -2172,7 +2174,7 @@
         <v>4</v>
       </c>
       <c r="C59" t="str">
-        <f>IF(D6&gt;0,"m_Matrix.mapLEDXY("&amp;A59&amp;","&amp;B59&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -2184,7 +2186,7 @@
         <v>5</v>
       </c>
       <c r="C60" t="str">
-        <f>IF(D7&gt;0,"m_Matrix.mapLEDXY("&amp;A60&amp;","&amp;B60&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -2244,7 +2246,7 @@
         <v>10</v>
       </c>
       <c r="C65" t="str">
-        <f>IF(D12&gt;0,"m_Matrix.mapLEDXY("&amp;A65&amp;","&amp;B65&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -2256,7 +2258,7 @@
         <v>11</v>
       </c>
       <c r="C66" t="str">
-        <f>IF(D13&gt;0,"m_Matrix.mapLEDXY("&amp;A66&amp;","&amp;B66&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -2268,7 +2270,7 @@
         <v>12</v>
       </c>
       <c r="C67" t="str">
-        <f>IF(D14&gt;0,"m_Matrix.mapLEDXY("&amp;A67&amp;","&amp;B67&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -2280,7 +2282,7 @@
         <v>13</v>
       </c>
       <c r="C68" t="str">
-        <f>IF(D15&gt;0,"m_Matrix.mapLEDXY("&amp;A68&amp;","&amp;B68&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -2292,7 +2294,7 @@
         <v>14</v>
       </c>
       <c r="C69" t="str">
-        <f>IF(D16&gt;0,"m_Matrix.mapLEDXY("&amp;A69&amp;","&amp;B69&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -2304,7 +2306,7 @@
         <v>15</v>
       </c>
       <c r="C70" t="str">
-        <f>IF(D17&gt;0,"m_Matrix.mapLEDXY("&amp;A70&amp;","&amp;B70&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -2316,7 +2318,7 @@
         <v>0</v>
       </c>
       <c r="C71" t="str">
-        <f>IF(E2&gt;0,"m_Matrix.mapLEDXY("&amp;A71&amp;","&amp;B71&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" ref="C71:C86" si="3">IF(E2&gt;0,"m_Matrix.mapLEDXY("&amp;A71&amp;","&amp;B71&amp;","&amp;$A$21&amp;");","")</f>
         <v/>
       </c>
     </row>
@@ -2328,7 +2330,7 @@
         <v>1</v>
       </c>
       <c r="C72" t="str">
-        <f>IF(E3&gt;0,"m_Matrix.mapLEDXY("&amp;A72&amp;","&amp;B72&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -2340,7 +2342,7 @@
         <v>2</v>
       </c>
       <c r="C73" t="str">
-        <f>IF(E4&gt;0,"m_Matrix.mapLEDXY("&amp;A73&amp;","&amp;B73&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -2352,7 +2354,7 @@
         <v>3</v>
       </c>
       <c r="C74" t="str">
-        <f>IF(E5&gt;0,"m_Matrix.mapLEDXY("&amp;A74&amp;","&amp;B74&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -2364,7 +2366,7 @@
         <v>4</v>
       </c>
       <c r="C75" t="str">
-        <f>IF(E6&gt;0,"m_Matrix.mapLEDXY("&amp;A75&amp;","&amp;B75&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -2376,7 +2378,7 @@
         <v>5</v>
       </c>
       <c r="C76" t="str">
-        <f>IF(E7&gt;0,"m_Matrix.mapLEDXY("&amp;A76&amp;","&amp;B76&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -2436,7 +2438,7 @@
         <v>10</v>
       </c>
       <c r="C81" t="str">
-        <f>IF(E12&gt;0,"m_Matrix.mapLEDXY("&amp;A81&amp;","&amp;B81&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -2448,7 +2450,7 @@
         <v>11</v>
       </c>
       <c r="C82" t="str">
-        <f>IF(E13&gt;0,"m_Matrix.mapLEDXY("&amp;A82&amp;","&amp;B82&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -2460,7 +2462,7 @@
         <v>12</v>
       </c>
       <c r="C83" t="str">
-        <f>IF(E14&gt;0,"m_Matrix.mapLEDXY("&amp;A83&amp;","&amp;B83&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -2472,7 +2474,7 @@
         <v>13</v>
       </c>
       <c r="C84" t="str">
-        <f>IF(E15&gt;0,"m_Matrix.mapLEDXY("&amp;A84&amp;","&amp;B84&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -2484,7 +2486,7 @@
         <v>14</v>
       </c>
       <c r="C85" t="str">
-        <f>IF(E16&gt;0,"m_Matrix.mapLEDXY("&amp;A85&amp;","&amp;B85&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -2496,7 +2498,7 @@
         <v>15</v>
       </c>
       <c r="C86" t="str">
-        <f>IF(E17&gt;0,"m_Matrix.mapLEDXY("&amp;A86&amp;","&amp;B86&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -2508,7 +2510,7 @@
         <v>0</v>
       </c>
       <c r="C87" t="str">
-        <f>IF(F2&gt;0,"m_Matrix.mapLEDXY("&amp;A87&amp;","&amp;B87&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" ref="C87:C102" si="4">IF(F2&gt;0,"m_Matrix.mapLEDXY("&amp;A87&amp;","&amp;B87&amp;","&amp;$A$21&amp;");","")</f>
         <v/>
       </c>
     </row>
@@ -2520,7 +2522,7 @@
         <v>1</v>
       </c>
       <c r="C88" t="str">
-        <f>IF(F3&gt;0,"m_Matrix.mapLEDXY("&amp;A88&amp;","&amp;B88&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -2532,7 +2534,7 @@
         <v>2</v>
       </c>
       <c r="C89" t="str">
-        <f>IF(F4&gt;0,"m_Matrix.mapLEDXY("&amp;A89&amp;","&amp;B89&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -2544,7 +2546,7 @@
         <v>3</v>
       </c>
       <c r="C90" t="str">
-        <f>IF(F5&gt;0,"m_Matrix.mapLEDXY("&amp;A90&amp;","&amp;B90&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -2556,7 +2558,7 @@
         <v>4</v>
       </c>
       <c r="C91" t="str">
-        <f>IF(F6&gt;0,"m_Matrix.mapLEDXY("&amp;A91&amp;","&amp;B91&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -2568,7 +2570,7 @@
         <v>5</v>
       </c>
       <c r="C92" t="str">
-        <f>IF(F7&gt;0,"m_Matrix.mapLEDXY("&amp;A92&amp;","&amp;B92&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -2628,7 +2630,7 @@
         <v>10</v>
       </c>
       <c r="C97" t="str">
-        <f>IF(F12&gt;0,"m_Matrix.mapLEDXY("&amp;A97&amp;","&amp;B97&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -2640,7 +2642,7 @@
         <v>11</v>
       </c>
       <c r="C98" t="str">
-        <f>IF(F13&gt;0,"m_Matrix.mapLEDXY("&amp;A98&amp;","&amp;B98&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -2652,7 +2654,7 @@
         <v>12</v>
       </c>
       <c r="C99" t="str">
-        <f>IF(F14&gt;0,"m_Matrix.mapLEDXY("&amp;A99&amp;","&amp;B99&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -2664,7 +2666,7 @@
         <v>13</v>
       </c>
       <c r="C100" t="str">
-        <f>IF(F15&gt;0,"m_Matrix.mapLEDXY("&amp;A100&amp;","&amp;B100&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -2676,7 +2678,7 @@
         <v>14</v>
       </c>
       <c r="C101" t="str">
-        <f>IF(F16&gt;0,"m_Matrix.mapLEDXY("&amp;A101&amp;","&amp;B101&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -2688,7 +2690,7 @@
         <v>15</v>
       </c>
       <c r="C102" t="str">
-        <f>IF(F17&gt;0,"m_Matrix.mapLEDXY("&amp;A102&amp;","&amp;B102&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -2700,7 +2702,7 @@
         <v>0</v>
       </c>
       <c r="C103" t="str">
-        <f>IF(G2&gt;0,"m_Matrix.mapLEDXY("&amp;A103&amp;","&amp;B103&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" ref="C103:C118" si="5">IF(G2&gt;0,"m_Matrix.mapLEDXY("&amp;A103&amp;","&amp;B103&amp;","&amp;$A$21&amp;");","")</f>
         <v/>
       </c>
     </row>
@@ -2712,7 +2714,7 @@
         <v>1</v>
       </c>
       <c r="C104" t="str">
-        <f>IF(G3&gt;0,"m_Matrix.mapLEDXY("&amp;A104&amp;","&amp;B104&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -2724,7 +2726,7 @@
         <v>2</v>
       </c>
       <c r="C105" t="str">
-        <f>IF(G4&gt;0,"m_Matrix.mapLEDXY("&amp;A105&amp;","&amp;B105&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -2736,7 +2738,7 @@
         <v>3</v>
       </c>
       <c r="C106" t="str">
-        <f>IF(G5&gt;0,"m_Matrix.mapLEDXY("&amp;A106&amp;","&amp;B106&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -2748,7 +2750,7 @@
         <v>4</v>
       </c>
       <c r="C107" t="str">
-        <f>IF(G6&gt;0,"m_Matrix.mapLEDXY("&amp;A107&amp;","&amp;B107&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -2760,7 +2762,7 @@
         <v>5</v>
       </c>
       <c r="C108" t="str">
-        <f>IF(G7&gt;0,"m_Matrix.mapLEDXY("&amp;A108&amp;","&amp;B108&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -2820,7 +2822,7 @@
         <v>10</v>
       </c>
       <c r="C113" t="str">
-        <f>IF(G12&gt;0,"m_Matrix.mapLEDXY("&amp;A113&amp;","&amp;B113&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -2832,7 +2834,7 @@
         <v>11</v>
       </c>
       <c r="C114" t="str">
-        <f>IF(G13&gt;0,"m_Matrix.mapLEDXY("&amp;A114&amp;","&amp;B114&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -2844,7 +2846,7 @@
         <v>12</v>
       </c>
       <c r="C115" t="str">
-        <f>IF(G14&gt;0,"m_Matrix.mapLEDXY("&amp;A115&amp;","&amp;B115&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -2856,7 +2858,7 @@
         <v>13</v>
       </c>
       <c r="C116" t="str">
-        <f>IF(G15&gt;0,"m_Matrix.mapLEDXY("&amp;A116&amp;","&amp;B116&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -2868,7 +2870,7 @@
         <v>14</v>
       </c>
       <c r="C117" t="str">
-        <f>IF(G16&gt;0,"m_Matrix.mapLEDXY("&amp;A117&amp;","&amp;B117&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -2880,7 +2882,7 @@
         <v>15</v>
       </c>
       <c r="C118" t="str">
-        <f>IF(G17&gt;0,"m_Matrix.mapLEDXY("&amp;A118&amp;","&amp;B118&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -2892,7 +2894,7 @@
         <v>0</v>
       </c>
       <c r="C119" t="str">
-        <f>IF(H2&gt;0,"m_Matrix.mapLEDXY("&amp;A119&amp;","&amp;B119&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" ref="C119:C134" si="6">IF(H2&gt;0,"m_Matrix.mapLEDXY("&amp;A119&amp;","&amp;B119&amp;","&amp;$A$21&amp;");","")</f>
         <v/>
       </c>
     </row>
@@ -2904,7 +2906,7 @@
         <v>1</v>
       </c>
       <c r="C120" t="str">
-        <f>IF(H3&gt;0,"m_Matrix.mapLEDXY("&amp;A120&amp;","&amp;B120&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -2916,7 +2918,7 @@
         <v>2</v>
       </c>
       <c r="C121" t="str">
-        <f>IF(H4&gt;0,"m_Matrix.mapLEDXY("&amp;A121&amp;","&amp;B121&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -2928,7 +2930,7 @@
         <v>3</v>
       </c>
       <c r="C122" t="str">
-        <f>IF(H5&gt;0,"m_Matrix.mapLEDXY("&amp;A122&amp;","&amp;B122&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -2940,7 +2942,7 @@
         <v>4</v>
       </c>
       <c r="C123" t="str">
-        <f>IF(H6&gt;0,"m_Matrix.mapLEDXY("&amp;A123&amp;","&amp;B123&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -2952,7 +2954,7 @@
         <v>5</v>
       </c>
       <c r="C124" t="str">
-        <f>IF(H7&gt;0,"m_Matrix.mapLEDXY("&amp;A124&amp;","&amp;B124&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -3012,7 +3014,7 @@
         <v>10</v>
       </c>
       <c r="C129" t="str">
-        <f>IF(H12&gt;0,"m_Matrix.mapLEDXY("&amp;A129&amp;","&amp;B129&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -3024,7 +3026,7 @@
         <v>11</v>
       </c>
       <c r="C130" t="str">
-        <f>IF(H13&gt;0,"m_Matrix.mapLEDXY("&amp;A130&amp;","&amp;B130&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -3036,7 +3038,7 @@
         <v>12</v>
       </c>
       <c r="C131" t="str">
-        <f>IF(H14&gt;0,"m_Matrix.mapLEDXY("&amp;A131&amp;","&amp;B131&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -3048,7 +3050,7 @@
         <v>13</v>
       </c>
       <c r="C132" t="str">
-        <f>IF(H15&gt;0,"m_Matrix.mapLEDXY("&amp;A132&amp;","&amp;B132&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -3060,7 +3062,7 @@
         <v>14</v>
       </c>
       <c r="C133" t="str">
-        <f>IF(H16&gt;0,"m_Matrix.mapLEDXY("&amp;A133&amp;","&amp;B133&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -3072,7 +3074,7 @@
         <v>15</v>
       </c>
       <c r="C134" t="str">
-        <f>IF(H17&gt;0,"m_Matrix.mapLEDXY("&amp;A134&amp;","&amp;B134&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -3084,7 +3086,7 @@
         <v>0</v>
       </c>
       <c r="C135" t="str">
-        <f>IF(I2&gt;0,"m_Matrix.mapLEDXY("&amp;A135&amp;","&amp;B135&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" ref="C135:C150" si="7">IF(I2&gt;0,"m_Matrix.mapLEDXY("&amp;A135&amp;","&amp;B135&amp;","&amp;$A$21&amp;");","")</f>
         <v/>
       </c>
     </row>
@@ -3096,7 +3098,7 @@
         <v>1</v>
       </c>
       <c r="C136" t="str">
-        <f>IF(I3&gt;0,"m_Matrix.mapLEDXY("&amp;A136&amp;","&amp;B136&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -3108,7 +3110,7 @@
         <v>2</v>
       </c>
       <c r="C137" t="str">
-        <f>IF(I4&gt;0,"m_Matrix.mapLEDXY("&amp;A137&amp;","&amp;B137&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -3120,7 +3122,7 @@
         <v>3</v>
       </c>
       <c r="C138" t="str">
-        <f>IF(I5&gt;0,"m_Matrix.mapLEDXY("&amp;A138&amp;","&amp;B138&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -3132,7 +3134,7 @@
         <v>4</v>
       </c>
       <c r="C139" t="str">
-        <f>IF(I6&gt;0,"m_Matrix.mapLEDXY("&amp;A139&amp;","&amp;B139&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -3144,7 +3146,7 @@
         <v>5</v>
       </c>
       <c r="C140" t="str">
-        <f>IF(I7&gt;0,"m_Matrix.mapLEDXY("&amp;A140&amp;","&amp;B140&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -3204,7 +3206,7 @@
         <v>10</v>
       </c>
       <c r="C145" t="str">
-        <f>IF(I12&gt;0,"m_Matrix.mapLEDXY("&amp;A145&amp;","&amp;B145&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -3216,7 +3218,7 @@
         <v>11</v>
       </c>
       <c r="C146" t="str">
-        <f>IF(I13&gt;0,"m_Matrix.mapLEDXY("&amp;A146&amp;","&amp;B146&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -3228,8 +3230,8 @@
         <v>12</v>
       </c>
       <c r="C147" t="str">
-        <f>IF(I14&gt;0,"m_Matrix.mapLEDXY("&amp;A147&amp;","&amp;B147&amp;","&amp;$A$21&amp;");","")</f>
-        <v>m_Matrix.mapLEDXY(7,12,mouthColor);</v>
+        <f t="shared" si="7"/>
+        <v/>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.5">
@@ -3240,7 +3242,7 @@
         <v>13</v>
       </c>
       <c r="C148" t="str">
-        <f>IF(I15&gt;0,"m_Matrix.mapLEDXY("&amp;A148&amp;","&amp;B148&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="7"/>
         <v>m_Matrix.mapLEDXY(7,13,mouthColor);</v>
       </c>
     </row>
@@ -3252,7 +3254,7 @@
         <v>14</v>
       </c>
       <c r="C149" t="str">
-        <f>IF(I16&gt;0,"m_Matrix.mapLEDXY("&amp;A149&amp;","&amp;B149&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -3264,7 +3266,7 @@
         <v>15</v>
       </c>
       <c r="C150" t="str">
-        <f>IF(I17&gt;0,"m_Matrix.mapLEDXY("&amp;A150&amp;","&amp;B150&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -3276,7 +3278,7 @@
         <v>0</v>
       </c>
       <c r="C151" t="str">
-        <f>IF(J2&gt;0,"m_Matrix.mapLEDXY("&amp;A151&amp;","&amp;B151&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" ref="C151:C166" si="8">IF(J2&gt;0,"m_Matrix.mapLEDXY("&amp;A151&amp;","&amp;B151&amp;","&amp;$A$21&amp;");","")</f>
         <v/>
       </c>
     </row>
@@ -3288,7 +3290,7 @@
         <v>1</v>
       </c>
       <c r="C152" t="str">
-        <f>IF(J3&gt;0,"m_Matrix.mapLEDXY("&amp;A152&amp;","&amp;B152&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -3300,7 +3302,7 @@
         <v>2</v>
       </c>
       <c r="C153" t="str">
-        <f>IF(J4&gt;0,"m_Matrix.mapLEDXY("&amp;A153&amp;","&amp;B153&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -3312,7 +3314,7 @@
         <v>3</v>
       </c>
       <c r="C154" t="str">
-        <f>IF(J5&gt;0,"m_Matrix.mapLEDXY("&amp;A154&amp;","&amp;B154&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -3324,7 +3326,7 @@
         <v>4</v>
       </c>
       <c r="C155" t="str">
-        <f>IF(J6&gt;0,"m_Matrix.mapLEDXY("&amp;A155&amp;","&amp;B155&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -3336,7 +3338,7 @@
         <v>5</v>
       </c>
       <c r="C156" t="str">
-        <f>IF(J7&gt;0,"m_Matrix.mapLEDXY("&amp;A156&amp;","&amp;B156&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -3396,7 +3398,7 @@
         <v>10</v>
       </c>
       <c r="C161" t="str">
-        <f>IF(J12&gt;0,"m_Matrix.mapLEDXY("&amp;A161&amp;","&amp;B161&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -3408,7 +3410,7 @@
         <v>11</v>
       </c>
       <c r="C162" t="str">
-        <f>IF(J13&gt;0,"m_Matrix.mapLEDXY("&amp;A162&amp;","&amp;B162&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -3420,8 +3422,8 @@
         <v>12</v>
       </c>
       <c r="C163" t="str">
-        <f>IF(J14&gt;0,"m_Matrix.mapLEDXY("&amp;A163&amp;","&amp;B163&amp;","&amp;$A$21&amp;");","")</f>
-        <v>m_Matrix.mapLEDXY(8,12,mouthColor);</v>
+        <f t="shared" si="8"/>
+        <v/>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.5">
@@ -3432,7 +3434,7 @@
         <v>13</v>
       </c>
       <c r="C164" t="str">
-        <f>IF(J15&gt;0,"m_Matrix.mapLEDXY("&amp;A164&amp;","&amp;B164&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="8"/>
         <v>m_Matrix.mapLEDXY(8,13,mouthColor);</v>
       </c>
     </row>
@@ -3444,7 +3446,7 @@
         <v>14</v>
       </c>
       <c r="C165" t="str">
-        <f>IF(J16&gt;0,"m_Matrix.mapLEDXY("&amp;A165&amp;","&amp;B165&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -3456,7 +3458,7 @@
         <v>15</v>
       </c>
       <c r="C166" t="str">
-        <f>IF(J17&gt;0,"m_Matrix.mapLEDXY("&amp;A166&amp;","&amp;B166&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -3468,7 +3470,7 @@
         <v>0</v>
       </c>
       <c r="C167" t="str">
-        <f>IF(K2&gt;0,"m_Matrix.mapLEDXY("&amp;A167&amp;","&amp;B167&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" ref="C167:C182" si="9">IF(K2&gt;0,"m_Matrix.mapLEDXY("&amp;A167&amp;","&amp;B167&amp;","&amp;$A$21&amp;");","")</f>
         <v/>
       </c>
     </row>
@@ -3480,7 +3482,7 @@
         <v>1</v>
       </c>
       <c r="C168" t="str">
-        <f>IF(K3&gt;0,"m_Matrix.mapLEDXY("&amp;A168&amp;","&amp;B168&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -3492,7 +3494,7 @@
         <v>2</v>
       </c>
       <c r="C169" t="str">
-        <f>IF(K4&gt;0,"m_Matrix.mapLEDXY("&amp;A169&amp;","&amp;B169&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -3504,7 +3506,7 @@
         <v>3</v>
       </c>
       <c r="C170" t="str">
-        <f>IF(K5&gt;0,"m_Matrix.mapLEDXY("&amp;A170&amp;","&amp;B170&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -3516,7 +3518,7 @@
         <v>4</v>
       </c>
       <c r="C171" t="str">
-        <f>IF(K6&gt;0,"m_Matrix.mapLEDXY("&amp;A171&amp;","&amp;B171&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -3528,7 +3530,7 @@
         <v>5</v>
       </c>
       <c r="C172" t="str">
-        <f>IF(K7&gt;0,"m_Matrix.mapLEDXY("&amp;A172&amp;","&amp;B172&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -3588,7 +3590,7 @@
         <v>10</v>
       </c>
       <c r="C177" t="str">
-        <f>IF(K12&gt;0,"m_Matrix.mapLEDXY("&amp;A177&amp;","&amp;B177&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -3600,7 +3602,7 @@
         <v>11</v>
       </c>
       <c r="C178" t="str">
-        <f>IF(K13&gt;0,"m_Matrix.mapLEDXY("&amp;A178&amp;","&amp;B178&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -3612,7 +3614,7 @@
         <v>12</v>
       </c>
       <c r="C179" t="str">
-        <f>IF(K14&gt;0,"m_Matrix.mapLEDXY("&amp;A179&amp;","&amp;B179&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -3624,7 +3626,7 @@
         <v>13</v>
       </c>
       <c r="C180" t="str">
-        <f>IF(K15&gt;0,"m_Matrix.mapLEDXY("&amp;A180&amp;","&amp;B180&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -3636,7 +3638,7 @@
         <v>14</v>
       </c>
       <c r="C181" t="str">
-        <f>IF(K16&gt;0,"m_Matrix.mapLEDXY("&amp;A181&amp;","&amp;B181&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -3648,7 +3650,7 @@
         <v>15</v>
       </c>
       <c r="C182" t="str">
-        <f>IF(K17&gt;0,"m_Matrix.mapLEDXY("&amp;A182&amp;","&amp;B182&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -3660,7 +3662,7 @@
         <v>0</v>
       </c>
       <c r="C183" t="str">
-        <f>IF(L2&gt;0,"m_Matrix.mapLEDXY("&amp;A183&amp;","&amp;B183&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" ref="C183:C198" si="10">IF(L2&gt;0,"m_Matrix.mapLEDXY("&amp;A183&amp;","&amp;B183&amp;","&amp;$A$21&amp;");","")</f>
         <v/>
       </c>
     </row>
@@ -3672,7 +3674,7 @@
         <v>1</v>
       </c>
       <c r="C184" t="str">
-        <f>IF(L3&gt;0,"m_Matrix.mapLEDXY("&amp;A184&amp;","&amp;B184&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
@@ -3684,7 +3686,7 @@
         <v>2</v>
       </c>
       <c r="C185" t="str">
-        <f>IF(L4&gt;0,"m_Matrix.mapLEDXY("&amp;A185&amp;","&amp;B185&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
@@ -3696,7 +3698,7 @@
         <v>3</v>
       </c>
       <c r="C186" t="str">
-        <f>IF(L5&gt;0,"m_Matrix.mapLEDXY("&amp;A186&amp;","&amp;B186&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
@@ -3708,7 +3710,7 @@
         <v>4</v>
       </c>
       <c r="C187" t="str">
-        <f>IF(L6&gt;0,"m_Matrix.mapLEDXY("&amp;A187&amp;","&amp;B187&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
@@ -3720,7 +3722,7 @@
         <v>5</v>
       </c>
       <c r="C188" t="str">
-        <f>IF(L7&gt;0,"m_Matrix.mapLEDXY("&amp;A188&amp;","&amp;B188&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
@@ -3780,7 +3782,7 @@
         <v>10</v>
       </c>
       <c r="C193" t="str">
-        <f>IF(L12&gt;0,"m_Matrix.mapLEDXY("&amp;A193&amp;","&amp;B193&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
@@ -3792,7 +3794,7 @@
         <v>11</v>
       </c>
       <c r="C194" t="str">
-        <f>IF(L13&gt;0,"m_Matrix.mapLEDXY("&amp;A194&amp;","&amp;B194&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
@@ -3804,7 +3806,7 @@
         <v>12</v>
       </c>
       <c r="C195" t="str">
-        <f>IF(L14&gt;0,"m_Matrix.mapLEDXY("&amp;A195&amp;","&amp;B195&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
@@ -3816,7 +3818,7 @@
         <v>13</v>
       </c>
       <c r="C196" t="str">
-        <f>IF(L15&gt;0,"m_Matrix.mapLEDXY("&amp;A196&amp;","&amp;B196&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
@@ -3828,7 +3830,7 @@
         <v>14</v>
       </c>
       <c r="C197" t="str">
-        <f>IF(L16&gt;0,"m_Matrix.mapLEDXY("&amp;A197&amp;","&amp;B197&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
@@ -3840,7 +3842,7 @@
         <v>15</v>
       </c>
       <c r="C198" t="str">
-        <f>IF(L17&gt;0,"m_Matrix.mapLEDXY("&amp;A198&amp;","&amp;B198&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
@@ -3852,7 +3854,7 @@
         <v>0</v>
       </c>
       <c r="C199" t="str">
-        <f>IF(M2&gt;0,"m_Matrix.mapLEDXY("&amp;A199&amp;","&amp;B199&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" ref="C199:C204" si="11">IF(M2&gt;0,"m_Matrix.mapLEDXY("&amp;A199&amp;","&amp;B199&amp;","&amp;$A$21&amp;");","")</f>
         <v/>
       </c>
     </row>
@@ -3864,7 +3866,7 @@
         <v>1</v>
       </c>
       <c r="C200" t="str">
-        <f>IF(M3&gt;0,"m_Matrix.mapLEDXY("&amp;A200&amp;","&amp;B200&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3876,7 +3878,7 @@
         <v>2</v>
       </c>
       <c r="C201" t="str">
-        <f>IF(M4&gt;0,"m_Matrix.mapLEDXY("&amp;A201&amp;","&amp;B201&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3888,7 +3890,7 @@
         <v>3</v>
       </c>
       <c r="C202" t="str">
-        <f>IF(M5&gt;0,"m_Matrix.mapLEDXY("&amp;A202&amp;","&amp;B202&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3900,7 +3902,7 @@
         <v>4</v>
       </c>
       <c r="C203" t="str">
-        <f>IF(M6&gt;0,"m_Matrix.mapLEDXY("&amp;A203&amp;","&amp;B203&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3912,7 +3914,7 @@
         <v>5</v>
       </c>
       <c r="C204" t="str">
-        <f>IF(M7&gt;0,"m_Matrix.mapLEDXY("&amp;A204&amp;","&amp;B204&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3971,7 +3973,7 @@
         <v>10</v>
       </c>
       <c r="C209" t="str">
-        <f>IF(M12&gt;0,"m_Matrix.mapLEDXY("&amp;A209&amp;","&amp;B209&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" ref="C209:C214" si="12">IF(M12&gt;0,"m_Matrix.mapLEDXY("&amp;A209&amp;","&amp;B209&amp;","&amp;$A$21&amp;");","")</f>
         <v/>
       </c>
     </row>
@@ -3983,7 +3985,7 @@
         <v>11</v>
       </c>
       <c r="C210" t="str">
-        <f>IF(M13&gt;0,"m_Matrix.mapLEDXY("&amp;A210&amp;","&amp;B210&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
     </row>
@@ -3995,7 +3997,7 @@
         <v>12</v>
       </c>
       <c r="C211" t="str">
-        <f>IF(M14&gt;0,"m_Matrix.mapLEDXY("&amp;A211&amp;","&amp;B211&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
     </row>
@@ -4007,7 +4009,7 @@
         <v>13</v>
       </c>
       <c r="C212" t="str">
-        <f>IF(M15&gt;0,"m_Matrix.mapLEDXY("&amp;A212&amp;","&amp;B212&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
     </row>
@@ -4019,7 +4021,7 @@
         <v>14</v>
       </c>
       <c r="C213" t="str">
-        <f>IF(M16&gt;0,"m_Matrix.mapLEDXY("&amp;A213&amp;","&amp;B213&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
     </row>
@@ -4031,7 +4033,7 @@
         <v>15</v>
       </c>
       <c r="C214" t="str">
-        <f>IF(M17&gt;0,"m_Matrix.mapLEDXY("&amp;A214&amp;","&amp;B214&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
     </row>
@@ -4043,7 +4045,7 @@
         <v>0</v>
       </c>
       <c r="C215" t="str">
-        <f>IF(N2&gt;0,"m_Matrix.mapLEDXY("&amp;A215&amp;","&amp;B215&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" ref="C215:C230" si="13">IF(N2&gt;0,"m_Matrix.mapLEDXY("&amp;A215&amp;","&amp;B215&amp;","&amp;$A$21&amp;");","")</f>
         <v/>
       </c>
     </row>
@@ -4055,7 +4057,7 @@
         <v>1</v>
       </c>
       <c r="C216" t="str">
-        <f>IF(N3&gt;0,"m_Matrix.mapLEDXY("&amp;A216&amp;","&amp;B216&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
@@ -4067,7 +4069,7 @@
         <v>2</v>
       </c>
       <c r="C217" t="str">
-        <f>IF(N4&gt;0,"m_Matrix.mapLEDXY("&amp;A217&amp;","&amp;B217&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
@@ -4079,7 +4081,7 @@
         <v>3</v>
       </c>
       <c r="C218" t="str">
-        <f>IF(N5&gt;0,"m_Matrix.mapLEDXY("&amp;A218&amp;","&amp;B218&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
@@ -4091,7 +4093,7 @@
         <v>4</v>
       </c>
       <c r="C219" t="str">
-        <f>IF(N6&gt;0,"m_Matrix.mapLEDXY("&amp;A219&amp;","&amp;B219&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
@@ -4103,7 +4105,7 @@
         <v>5</v>
       </c>
       <c r="C220" t="str">
-        <f>IF(N7&gt;0,"m_Matrix.mapLEDXY("&amp;A220&amp;","&amp;B220&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
@@ -4163,7 +4165,7 @@
         <v>10</v>
       </c>
       <c r="C225" t="str">
-        <f>IF(N12&gt;0,"m_Matrix.mapLEDXY("&amp;A225&amp;","&amp;B225&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
@@ -4175,7 +4177,7 @@
         <v>11</v>
       </c>
       <c r="C226" t="str">
-        <f>IF(N13&gt;0,"m_Matrix.mapLEDXY("&amp;A226&amp;","&amp;B226&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
@@ -4187,7 +4189,7 @@
         <v>12</v>
       </c>
       <c r="C227" t="str">
-        <f>IF(N14&gt;0,"m_Matrix.mapLEDXY("&amp;A227&amp;","&amp;B227&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
@@ -4199,7 +4201,7 @@
         <v>13</v>
       </c>
       <c r="C228" t="str">
-        <f>IF(N15&gt;0,"m_Matrix.mapLEDXY("&amp;A228&amp;","&amp;B228&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
@@ -4211,7 +4213,7 @@
         <v>14</v>
       </c>
       <c r="C229" t="str">
-        <f>IF(N16&gt;0,"m_Matrix.mapLEDXY("&amp;A229&amp;","&amp;B229&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
@@ -4223,7 +4225,7 @@
         <v>15</v>
       </c>
       <c r="C230" t="str">
-        <f>IF(N17&gt;0,"m_Matrix.mapLEDXY("&amp;A230&amp;","&amp;B230&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
@@ -4235,7 +4237,7 @@
         <v>0</v>
       </c>
       <c r="C231" t="str">
-        <f>IF(O2&gt;0,"m_Matrix.mapLEDXY("&amp;A231&amp;","&amp;B231&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" ref="C231:C246" si="14">IF(O2&gt;0,"m_Matrix.mapLEDXY("&amp;A231&amp;","&amp;B231&amp;","&amp;$A$21&amp;");","")</f>
         <v/>
       </c>
     </row>
@@ -4247,7 +4249,7 @@
         <v>1</v>
       </c>
       <c r="C232" t="str">
-        <f>IF(O3&gt;0,"m_Matrix.mapLEDXY("&amp;A232&amp;","&amp;B232&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
@@ -4259,7 +4261,7 @@
         <v>2</v>
       </c>
       <c r="C233" t="str">
-        <f>IF(O4&gt;0,"m_Matrix.mapLEDXY("&amp;A233&amp;","&amp;B233&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
@@ -4271,7 +4273,7 @@
         <v>3</v>
       </c>
       <c r="C234" t="str">
-        <f>IF(O5&gt;0,"m_Matrix.mapLEDXY("&amp;A234&amp;","&amp;B234&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
@@ -4283,7 +4285,7 @@
         <v>4</v>
       </c>
       <c r="C235" t="str">
-        <f>IF(O6&gt;0,"m_Matrix.mapLEDXY("&amp;A235&amp;","&amp;B235&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
@@ -4295,7 +4297,7 @@
         <v>5</v>
       </c>
       <c r="C236" t="str">
-        <f>IF(O7&gt;0,"m_Matrix.mapLEDXY("&amp;A236&amp;","&amp;B236&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
@@ -4355,7 +4357,7 @@
         <v>10</v>
       </c>
       <c r="C241" t="str">
-        <f>IF(O12&gt;0,"m_Matrix.mapLEDXY("&amp;A241&amp;","&amp;B241&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
@@ -4367,7 +4369,7 @@
         <v>11</v>
       </c>
       <c r="C242" t="str">
-        <f>IF(O13&gt;0,"m_Matrix.mapLEDXY("&amp;A242&amp;","&amp;B242&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
@@ -4379,7 +4381,7 @@
         <v>12</v>
       </c>
       <c r="C243" t="str">
-        <f>IF(O14&gt;0,"m_Matrix.mapLEDXY("&amp;A243&amp;","&amp;B243&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
@@ -4391,7 +4393,7 @@
         <v>13</v>
       </c>
       <c r="C244" t="str">
-        <f>IF(O15&gt;0,"m_Matrix.mapLEDXY("&amp;A244&amp;","&amp;B244&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
@@ -4403,7 +4405,7 @@
         <v>14</v>
       </c>
       <c r="C245" t="str">
-        <f>IF(O16&gt;0,"m_Matrix.mapLEDXY("&amp;A245&amp;","&amp;B245&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
@@ -4415,7 +4417,7 @@
         <v>15</v>
       </c>
       <c r="C246" t="str">
-        <f>IF(O17&gt;0,"m_Matrix.mapLEDXY("&amp;A246&amp;","&amp;B246&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
@@ -4427,7 +4429,7 @@
         <v>0</v>
       </c>
       <c r="C247" t="str">
-        <f>IF(P2&gt;0,"m_Matrix.mapLEDXY("&amp;A247&amp;","&amp;B247&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" ref="C247:C262" si="15">IF(P2&gt;0,"m_Matrix.mapLEDXY("&amp;A247&amp;","&amp;B247&amp;","&amp;$A$21&amp;");","")</f>
         <v/>
       </c>
     </row>
@@ -4439,7 +4441,7 @@
         <v>1</v>
       </c>
       <c r="C248" t="str">
-        <f>IF(P3&gt;0,"m_Matrix.mapLEDXY("&amp;A248&amp;","&amp;B248&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
@@ -4451,7 +4453,7 @@
         <v>2</v>
       </c>
       <c r="C249" t="str">
-        <f>IF(P4&gt;0,"m_Matrix.mapLEDXY("&amp;A249&amp;","&amp;B249&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
@@ -4463,7 +4465,7 @@
         <v>3</v>
       </c>
       <c r="C250" t="str">
-        <f>IF(P5&gt;0,"m_Matrix.mapLEDXY("&amp;A250&amp;","&amp;B250&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
@@ -4475,7 +4477,7 @@
         <v>4</v>
       </c>
       <c r="C251" t="str">
-        <f>IF(P6&gt;0,"m_Matrix.mapLEDXY("&amp;A251&amp;","&amp;B251&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
@@ -4487,7 +4489,7 @@
         <v>5</v>
       </c>
       <c r="C252" t="str">
-        <f>IF(P7&gt;0,"m_Matrix.mapLEDXY("&amp;A252&amp;","&amp;B252&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
@@ -4499,7 +4501,7 @@
         <v>6</v>
       </c>
       <c r="C253" t="str">
-        <f>IF(P8&gt;0,"m_Matrix.mapLEDXY("&amp;A253&amp;","&amp;B253&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
@@ -4511,7 +4513,7 @@
         <v>7</v>
       </c>
       <c r="C254" t="str">
-        <f>IF(P9&gt;0,"m_Matrix.mapLEDXY("&amp;A254&amp;","&amp;B254&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
@@ -4523,7 +4525,7 @@
         <v>8</v>
       </c>
       <c r="C255" t="str">
-        <f>IF(P10&gt;0,"m_Matrix.mapLEDXY("&amp;A255&amp;","&amp;B255&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
@@ -4535,7 +4537,7 @@
         <v>9</v>
       </c>
       <c r="C256" t="str">
-        <f>IF(P11&gt;0,"m_Matrix.mapLEDXY("&amp;A256&amp;","&amp;B256&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
@@ -4547,7 +4549,7 @@
         <v>10</v>
       </c>
       <c r="C257" t="str">
-        <f>IF(P12&gt;0,"m_Matrix.mapLEDXY("&amp;A257&amp;","&amp;B257&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
@@ -4559,7 +4561,7 @@
         <v>11</v>
       </c>
       <c r="C258" t="str">
-        <f>IF(P13&gt;0,"m_Matrix.mapLEDXY("&amp;A258&amp;","&amp;B258&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
@@ -4571,7 +4573,7 @@
         <v>12</v>
       </c>
       <c r="C259" t="str">
-        <f>IF(P14&gt;0,"m_Matrix.mapLEDXY("&amp;A259&amp;","&amp;B259&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
@@ -4583,7 +4585,7 @@
         <v>13</v>
       </c>
       <c r="C260" t="str">
-        <f>IF(P15&gt;0,"m_Matrix.mapLEDXY("&amp;A260&amp;","&amp;B260&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
@@ -4595,7 +4597,7 @@
         <v>14</v>
       </c>
       <c r="C261" t="str">
-        <f>IF(P16&gt;0,"m_Matrix.mapLEDXY("&amp;A261&amp;","&amp;B261&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
@@ -4607,7 +4609,7 @@
         <v>15</v>
       </c>
       <c r="C262" t="str">
-        <f>IF(P17&gt;0,"m_Matrix.mapLEDXY("&amp;A262&amp;","&amp;B262&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
@@ -4619,7 +4621,7 @@
         <v>0</v>
       </c>
       <c r="C263" t="str">
-        <f>IF(Q2&gt;0,"m_Matrix.mapLEDXY("&amp;A263&amp;","&amp;B263&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" ref="C263:C278" si="16">IF(Q2&gt;0,"m_Matrix.mapLEDXY("&amp;A263&amp;","&amp;B263&amp;","&amp;$A$21&amp;");","")</f>
         <v/>
       </c>
     </row>
@@ -4631,7 +4633,7 @@
         <v>1</v>
       </c>
       <c r="C264" t="str">
-        <f>IF(Q3&gt;0,"m_Matrix.mapLEDXY("&amp;A264&amp;","&amp;B264&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -4643,7 +4645,7 @@
         <v>2</v>
       </c>
       <c r="C265" t="str">
-        <f>IF(Q4&gt;0,"m_Matrix.mapLEDXY("&amp;A265&amp;","&amp;B265&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -4655,7 +4657,7 @@
         <v>3</v>
       </c>
       <c r="C266" t="str">
-        <f>IF(Q5&gt;0,"m_Matrix.mapLEDXY("&amp;A266&amp;","&amp;B266&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -4667,7 +4669,7 @@
         <v>4</v>
       </c>
       <c r="C267" t="str">
-        <f>IF(Q6&gt;0,"m_Matrix.mapLEDXY("&amp;A267&amp;","&amp;B267&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -4679,7 +4681,7 @@
         <v>5</v>
       </c>
       <c r="C268" t="str">
-        <f>IF(Q7&gt;0,"m_Matrix.mapLEDXY("&amp;A268&amp;","&amp;B268&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -4691,7 +4693,7 @@
         <v>6</v>
       </c>
       <c r="C269" t="str">
-        <f>IF(Q8&gt;0,"m_Matrix.mapLEDXY("&amp;A269&amp;","&amp;B269&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -4703,7 +4705,7 @@
         <v>7</v>
       </c>
       <c r="C270" t="str">
-        <f>IF(Q9&gt;0,"m_Matrix.mapLEDXY("&amp;A270&amp;","&amp;B270&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -4715,7 +4717,7 @@
         <v>8</v>
       </c>
       <c r="C271" t="str">
-        <f>IF(Q10&gt;0,"m_Matrix.mapLEDXY("&amp;A271&amp;","&amp;B271&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -4727,7 +4729,7 @@
         <v>9</v>
       </c>
       <c r="C272" t="str">
-        <f>IF(Q11&gt;0,"m_Matrix.mapLEDXY("&amp;A272&amp;","&amp;B272&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -4739,7 +4741,7 @@
         <v>10</v>
       </c>
       <c r="C273" t="str">
-        <f>IF(Q12&gt;0,"m_Matrix.mapLEDXY("&amp;A273&amp;","&amp;B273&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -4751,7 +4753,7 @@
         <v>11</v>
       </c>
       <c r="C274" t="str">
-        <f>IF(Q13&gt;0,"m_Matrix.mapLEDXY("&amp;A274&amp;","&amp;B274&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -4763,7 +4765,7 @@
         <v>12</v>
       </c>
       <c r="C275" t="str">
-        <f>IF(Q14&gt;0,"m_Matrix.mapLEDXY("&amp;A275&amp;","&amp;B275&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -4775,7 +4777,7 @@
         <v>13</v>
       </c>
       <c r="C276" t="str">
-        <f>IF(Q15&gt;0,"m_Matrix.mapLEDXY("&amp;A276&amp;","&amp;B276&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -4787,7 +4789,7 @@
         <v>14</v>
       </c>
       <c r="C277" t="str">
-        <f>IF(Q16&gt;0,"m_Matrix.mapLEDXY("&amp;A277&amp;","&amp;B277&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -4799,7 +4801,7 @@
         <v>15</v>
       </c>
       <c r="C278" t="str">
-        <f>IF(Q17&gt;0,"m_Matrix.mapLEDXY("&amp;A278&amp;","&amp;B278&amp;","&amp;$A$21&amp;");","")</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>

</xml_diff>